<commit_message>
validation of decoder functionality with all instructions
</commit_message>
<xml_diff>
--- a/RTL/ControlUnit/Instructions.xlsx
+++ b/RTL/ControlUnit/Instructions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Noah\Dokumente\Code\EDRICO\EDRICO\RTL\ControlUnit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BEAED40-173B-42F8-8CE4-F0D74A4C87F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1CA8CE-A78D-4A17-9674-677D81F38657}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14835" yWindow="1410" windowWidth="21600" windowHeight="11385" xr2:uid="{1564D8D6-0412-4888-BC3B-BF158BBB57A2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1564D8D6-0412-4888-BC3B-BF158BBB57A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>BIT</t>
   </si>
@@ -138,16 +138,22 @@
     <t>CSRRWI</t>
   </si>
   <si>
-    <t>iie???</t>
+    <t>LB</t>
   </si>
   <si>
-    <t>wrong imm, wrong A_MUX</t>
+    <t>LH</t>
   </si>
   <si>
-    <t>type_of instr. Wrong</t>
+    <t>LW</t>
   </si>
   <si>
-    <t>TOI not set correctly?!?!??! Why A_MUX = 01?</t>
+    <t>SB</t>
+  </si>
+  <si>
+    <t>SH</t>
+  </si>
+  <si>
+    <t>SW</t>
   </si>
 </sst>
 </file>
@@ -176,7 +182,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -191,19 +197,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -285,7 +279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -293,8 +287,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -316,11 +308,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
@@ -372,7 +364,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp22.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp23.xml><?xml version="1.0" encoding="utf-8"?>
@@ -380,27 +372,27 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp24.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp25.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp26.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp27.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp28.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp29.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -408,15 +400,15 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp30.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp31.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp32.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2092,7 +2084,7 @@
           <xdr:col>34</xdr:col>
           <xdr:colOff>495300</xdr:colOff>
           <xdr:row>26</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2177,8 +2169,8 @@
         <xdr:to>
           <xdr:col>34</xdr:col>
           <xdr:colOff>495300</xdr:colOff>
-          <xdr:row>27</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:row>26</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2263,8 +2255,8 @@
         <xdr:to>
           <xdr:col>34</xdr:col>
           <xdr:colOff>495300</xdr:colOff>
-          <xdr:row>28</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:row>27</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2436,7 +2428,7 @@
           <xdr:col>34</xdr:col>
           <xdr:colOff>476250</xdr:colOff>
           <xdr:row>31</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2607,8 +2599,8 @@
         <xdr:to>
           <xdr:col>34</xdr:col>
           <xdr:colOff>485775</xdr:colOff>
-          <xdr:row>34</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:row>33</xdr:row>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2780,7 +2772,7 @@
           <xdr:col>34</xdr:col>
           <xdr:colOff>523875</xdr:colOff>
           <xdr:row>39</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2952,7 +2944,7 @@
           <xdr:col>34</xdr:col>
           <xdr:colOff>523875</xdr:colOff>
           <xdr:row>41</xdr:row>
-          <xdr:rowOff>180975</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3038,7 +3030,7 @@
           <xdr:col>34</xdr:col>
           <xdr:colOff>533400</xdr:colOff>
           <xdr:row>43</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3124,7 +3116,7 @@
           <xdr:col>34</xdr:col>
           <xdr:colOff>504825</xdr:colOff>
           <xdr:row>37</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3497,10 +3489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89A24D75-4A62-4BD0-ADC9-1AF25F8BE728}">
-  <dimension ref="A4:AI43"/>
+  <dimension ref="A4:AG51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q4" workbookViewId="0">
-      <selection activeCell="AI20" sqref="AI20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="AI44" sqref="AI44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3509,46 +3501,46 @@
     <col min="35" max="35" width="29.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="9"/>
-      <c r="S4" s="9"/>
-      <c r="T4" s="9"/>
-      <c r="U4" s="9"/>
-      <c r="V4" s="9"/>
-      <c r="W4" s="9"/>
-      <c r="X4" s="9"/>
-      <c r="Y4" s="9"/>
-      <c r="Z4" s="9"/>
-      <c r="AA4" s="9"/>
-      <c r="AB4" s="9"/>
-      <c r="AC4" s="9"/>
-      <c r="AD4" s="9"/>
-      <c r="AE4" s="9"/>
-      <c r="AF4" s="9"/>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="7"/>
+      <c r="Y4" s="7"/>
+      <c r="Z4" s="7"/>
+      <c r="AA4" s="7"/>
+      <c r="AB4" s="7"/>
+      <c r="AC4" s="7"/>
+      <c r="AD4" s="7"/>
+      <c r="AE4" s="7"/>
+      <c r="AF4" s="7"/>
       <c r="AG4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>31</v>
       </c>
@@ -3646,7 +3638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>0</v>
       </c>
@@ -3746,11 +3738,8 @@
       <c r="AG6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="AI6" t="s">
-        <v>34</v>
-      </c>
     </row>
-    <row r="7" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>0</v>
       </c>
@@ -3847,11 +3836,11 @@
       <c r="AF7" s="2">
         <v>1</v>
       </c>
-      <c r="AG7" s="7" t="s">
+      <c r="AG7" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>0</v>
       </c>
@@ -3948,11 +3937,11 @@
       <c r="AF8" s="2">
         <v>1</v>
       </c>
-      <c r="AG8" s="7" t="s">
+      <c r="AG8" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>0</v>
       </c>
@@ -4049,11 +4038,11 @@
       <c r="AF9" s="2">
         <v>1</v>
       </c>
-      <c r="AG9" s="7" t="s">
+      <c r="AG9" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>0</v>
       </c>
@@ -4150,11 +4139,11 @@
       <c r="AF10" s="2">
         <v>1</v>
       </c>
-      <c r="AG10" s="7" t="s">
+      <c r="AG10" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>0</v>
       </c>
@@ -4251,11 +4240,11 @@
       <c r="AF11" s="2">
         <v>1</v>
       </c>
-      <c r="AG11" s="7" t="s">
+      <c r="AG11" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>0</v>
       </c>
@@ -4352,11 +4341,11 @@
       <c r="AF12" s="2">
         <v>1</v>
       </c>
-      <c r="AG12" s="7" t="s">
+      <c r="AG12" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>0</v>
       </c>
@@ -4453,11 +4442,11 @@
       <c r="AF13" s="2">
         <v>1</v>
       </c>
-      <c r="AG13" s="7" t="s">
+      <c r="AG13" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>0</v>
       </c>
@@ -4554,11 +4543,11 @@
       <c r="AF14" s="2">
         <v>1</v>
       </c>
-      <c r="AG14" s="7" t="s">
+      <c r="AG14" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>0</v>
       </c>
@@ -4658,11 +4647,8 @@
       <c r="AG15" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="AI15" t="s">
-        <v>35</v>
-      </c>
     </row>
-    <row r="16" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>0</v>
       </c>
@@ -4759,11 +4745,11 @@
       <c r="AF16" s="2">
         <v>1</v>
       </c>
-      <c r="AG16" t="s">
+      <c r="AG16" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>0</v>
       </c>
@@ -4860,11 +4846,11 @@
       <c r="AF17" s="2">
         <v>1</v>
       </c>
-      <c r="AG17" t="s">
+      <c r="AG17" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>0</v>
       </c>
@@ -4961,11 +4947,11 @@
       <c r="AF18" s="2">
         <v>1</v>
       </c>
-      <c r="AG18" t="s">
+      <c r="AG18" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>0</v>
       </c>
@@ -5062,11 +5048,11 @@
       <c r="AF19" s="2">
         <v>1</v>
       </c>
-      <c r="AG19" t="s">
+      <c r="AG19" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>0</v>
       </c>
@@ -5163,11 +5149,11 @@
       <c r="AF20" s="2">
         <v>1</v>
       </c>
-      <c r="AG20" t="s">
+      <c r="AG20" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>0</v>
       </c>
@@ -5264,11 +5250,11 @@
       <c r="AF21" s="2">
         <v>1</v>
       </c>
-      <c r="AG21" t="s">
+      <c r="AG21" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>0</v>
       </c>
@@ -5365,11 +5351,11 @@
       <c r="AF22" s="2">
         <v>1</v>
       </c>
-      <c r="AG22" t="s">
+      <c r="AG22" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>0</v>
       </c>
@@ -5466,11 +5452,11 @@
       <c r="AF23" s="2">
         <v>1</v>
       </c>
-      <c r="AG23" t="s">
+      <c r="AG23" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>0</v>
       </c>
@@ -5567,1327 +5553,1951 @@
       <c r="AF24" s="5">
         <v>1</v>
       </c>
-      <c r="AG24" t="s">
+      <c r="AG24" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>0</v>
-      </c>
-      <c r="B26">
-        <v>0</v>
-      </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
-      <c r="H26">
-        <v>0</v>
-      </c>
-      <c r="I26">
-        <v>0</v>
-      </c>
-      <c r="J26">
-        <v>0</v>
-      </c>
-      <c r="K26">
-        <v>0</v>
-      </c>
-      <c r="L26">
-        <v>0</v>
-      </c>
-      <c r="M26">
-        <v>0</v>
-      </c>
-      <c r="N26">
-        <v>0</v>
-      </c>
-      <c r="O26">
-        <v>0</v>
-      </c>
-      <c r="P26">
-        <v>0</v>
-      </c>
-      <c r="Q26">
-        <v>0</v>
-      </c>
-      <c r="R26">
-        <v>1</v>
-      </c>
-      <c r="S26">
-        <v>1</v>
-      </c>
-      <c r="T26">
-        <v>1</v>
-      </c>
-      <c r="U26">
-        <v>0</v>
-      </c>
-      <c r="V26">
-        <v>0</v>
-      </c>
-      <c r="W26">
-        <v>0</v>
-      </c>
-      <c r="X26">
-        <v>0</v>
-      </c>
-      <c r="Y26">
-        <v>1</v>
-      </c>
-      <c r="Z26">
-        <v>0</v>
-      </c>
-      <c r="AA26">
-        <v>1</v>
-      </c>
-      <c r="AB26">
-        <v>1</v>
-      </c>
-      <c r="AC26">
-        <v>0</v>
-      </c>
-      <c r="AD26">
-        <v>1</v>
-      </c>
-      <c r="AE26">
-        <v>1</v>
-      </c>
-      <c r="AF26">
-        <v>1</v>
-      </c>
-      <c r="AG26" t="s">
+    <row r="25" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AG25" s="6"/>
+    </row>
+    <row r="26" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>0</v>
+      </c>
+      <c r="B26" s="2">
+        <v>0</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0</v>
+      </c>
+      <c r="G26" s="2">
+        <v>0</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0</v>
+      </c>
+      <c r="I26" s="2">
+        <v>0</v>
+      </c>
+      <c r="J26" s="2">
+        <v>0</v>
+      </c>
+      <c r="K26" s="2">
+        <v>0</v>
+      </c>
+      <c r="L26" s="2">
+        <v>0</v>
+      </c>
+      <c r="M26" s="2">
+        <v>0</v>
+      </c>
+      <c r="N26" s="2">
+        <v>0</v>
+      </c>
+      <c r="O26" s="2">
+        <v>0</v>
+      </c>
+      <c r="P26" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="2">
+        <v>0</v>
+      </c>
+      <c r="R26" s="2">
+        <v>1</v>
+      </c>
+      <c r="S26" s="2">
+        <v>1</v>
+      </c>
+      <c r="T26" s="2">
+        <v>1</v>
+      </c>
+      <c r="U26" s="2">
+        <v>0</v>
+      </c>
+      <c r="V26" s="2">
+        <v>0</v>
+      </c>
+      <c r="W26" s="2">
+        <v>0</v>
+      </c>
+      <c r="X26" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y26" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z26" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA26" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB26" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC26" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD26" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE26" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF26" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG26" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>0</v>
-      </c>
-      <c r="B27">
-        <v>0</v>
-      </c>
-      <c r="C27">
-        <v>0</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
-      <c r="I27">
-        <v>0</v>
-      </c>
-      <c r="J27">
-        <v>0</v>
-      </c>
-      <c r="K27">
-        <v>0</v>
-      </c>
-      <c r="L27">
-        <v>0</v>
-      </c>
-      <c r="M27">
-        <v>0</v>
-      </c>
-      <c r="N27">
-        <v>0</v>
-      </c>
-      <c r="O27">
-        <v>0</v>
-      </c>
-      <c r="P27">
-        <v>0</v>
-      </c>
-      <c r="Q27">
-        <v>0</v>
-      </c>
-      <c r="R27">
-        <v>1</v>
-      </c>
-      <c r="S27">
-        <v>1</v>
-      </c>
-      <c r="T27">
-        <v>1</v>
-      </c>
-      <c r="U27">
-        <v>0</v>
-      </c>
-      <c r="V27">
-        <v>0</v>
-      </c>
-      <c r="W27">
-        <v>0</v>
-      </c>
-      <c r="X27">
-        <v>0</v>
-      </c>
-      <c r="Y27">
-        <v>1</v>
-      </c>
-      <c r="Z27">
-        <v>0</v>
-      </c>
-      <c r="AA27">
-        <v>0</v>
-      </c>
-      <c r="AB27">
-        <v>1</v>
-      </c>
-      <c r="AC27">
-        <v>0</v>
-      </c>
-      <c r="AD27">
-        <v>1</v>
-      </c>
-      <c r="AE27">
-        <v>1</v>
-      </c>
-      <c r="AF27">
-        <v>1</v>
-      </c>
-      <c r="AG27" t="s">
+    <row r="27" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>0</v>
+      </c>
+      <c r="B27" s="2">
+        <v>0</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0</v>
+      </c>
+      <c r="H27" s="2">
+        <v>0</v>
+      </c>
+      <c r="I27" s="2">
+        <v>0</v>
+      </c>
+      <c r="J27" s="2">
+        <v>0</v>
+      </c>
+      <c r="K27" s="2">
+        <v>0</v>
+      </c>
+      <c r="L27" s="2">
+        <v>0</v>
+      </c>
+      <c r="M27" s="2">
+        <v>0</v>
+      </c>
+      <c r="N27" s="2">
+        <v>0</v>
+      </c>
+      <c r="O27" s="2">
+        <v>0</v>
+      </c>
+      <c r="P27" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="2">
+        <v>0</v>
+      </c>
+      <c r="R27" s="2">
+        <v>1</v>
+      </c>
+      <c r="S27" s="2">
+        <v>1</v>
+      </c>
+      <c r="T27" s="2">
+        <v>1</v>
+      </c>
+      <c r="U27" s="2">
+        <v>0</v>
+      </c>
+      <c r="V27" s="2">
+        <v>0</v>
+      </c>
+      <c r="W27" s="2">
+        <v>0</v>
+      </c>
+      <c r="X27" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y27" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z27" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA27" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB27" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC27" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD27" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE27" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF27" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG27" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>0</v>
-      </c>
-      <c r="B28">
-        <v>0</v>
-      </c>
-      <c r="C28">
-        <v>0</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-      <c r="F28">
-        <v>1</v>
-      </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
-      <c r="H28">
-        <v>0</v>
-      </c>
-      <c r="I28">
-        <v>0</v>
-      </c>
-      <c r="J28">
-        <v>0</v>
-      </c>
-      <c r="K28">
-        <v>0</v>
-      </c>
-      <c r="L28">
-        <v>1</v>
-      </c>
-      <c r="M28">
-        <v>0</v>
-      </c>
-      <c r="N28">
-        <v>0</v>
-      </c>
-      <c r="O28">
-        <v>0</v>
-      </c>
-      <c r="P28">
-        <v>0</v>
-      </c>
-      <c r="Q28">
-        <v>1</v>
-      </c>
-      <c r="R28">
-        <v>0</v>
-      </c>
-      <c r="S28">
-        <v>0</v>
-      </c>
-      <c r="T28">
-        <v>1</v>
-      </c>
-      <c r="U28">
-        <v>0</v>
-      </c>
-      <c r="V28">
-        <v>0</v>
-      </c>
-      <c r="W28">
-        <v>0</v>
-      </c>
-      <c r="X28">
-        <v>0</v>
-      </c>
-      <c r="Y28">
-        <v>1</v>
-      </c>
-      <c r="Z28">
-        <v>1</v>
-      </c>
-      <c r="AA28">
-        <v>1</v>
-      </c>
-      <c r="AB28">
-        <v>0</v>
-      </c>
-      <c r="AC28">
-        <v>1</v>
-      </c>
-      <c r="AD28">
-        <v>1</v>
-      </c>
-      <c r="AE28">
-        <v>1</v>
-      </c>
-      <c r="AF28">
-        <v>1</v>
-      </c>
-      <c r="AG28" s="8" t="s">
+    <row r="28" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <v>0</v>
+      </c>
+      <c r="B28" s="2">
+        <v>0</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0</v>
+      </c>
+      <c r="F28" s="2">
+        <v>1</v>
+      </c>
+      <c r="G28" s="2">
+        <v>0</v>
+      </c>
+      <c r="H28" s="2">
+        <v>0</v>
+      </c>
+      <c r="I28" s="2">
+        <v>0</v>
+      </c>
+      <c r="J28" s="2">
+        <v>0</v>
+      </c>
+      <c r="K28" s="2">
+        <v>0</v>
+      </c>
+      <c r="L28" s="2">
+        <v>1</v>
+      </c>
+      <c r="M28" s="2">
+        <v>0</v>
+      </c>
+      <c r="N28" s="2">
+        <v>0</v>
+      </c>
+      <c r="O28" s="2">
+        <v>0</v>
+      </c>
+      <c r="P28" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="2">
+        <v>1</v>
+      </c>
+      <c r="R28" s="2">
+        <v>0</v>
+      </c>
+      <c r="S28" s="2">
+        <v>0</v>
+      </c>
+      <c r="T28" s="2">
+        <v>1</v>
+      </c>
+      <c r="U28" s="2">
+        <v>0</v>
+      </c>
+      <c r="V28" s="2">
+        <v>0</v>
+      </c>
+      <c r="W28" s="2">
+        <v>0</v>
+      </c>
+      <c r="X28" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y28" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z28" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA28" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB28" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC28" s="2">
+        <v>1</v>
+      </c>
+      <c r="AD28" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE28" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF28" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG28" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="AI28" t="s">
-        <v>37</v>
-      </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>0</v>
-      </c>
-      <c r="B29">
-        <v>0</v>
-      </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="G29">
-        <v>1</v>
-      </c>
-      <c r="H29">
-        <v>0</v>
-      </c>
-      <c r="I29">
-        <v>1</v>
-      </c>
-      <c r="J29">
-        <v>0</v>
-      </c>
-      <c r="K29">
-        <v>1</v>
-      </c>
-      <c r="L29">
-        <v>0</v>
-      </c>
-      <c r="M29">
-        <v>0</v>
-      </c>
-      <c r="N29">
-        <v>0</v>
-      </c>
-      <c r="O29">
-        <v>1</v>
-      </c>
-      <c r="P29">
-        <v>0</v>
-      </c>
-      <c r="Q29">
-        <v>0</v>
-      </c>
-      <c r="R29">
-        <v>0</v>
-      </c>
-      <c r="S29">
-        <v>0</v>
-      </c>
-      <c r="T29">
-        <v>0</v>
-      </c>
-      <c r="U29">
-        <v>0</v>
-      </c>
-      <c r="V29">
-        <v>0</v>
-      </c>
-      <c r="W29">
-        <v>0</v>
-      </c>
-      <c r="X29">
-        <v>0</v>
-      </c>
-      <c r="Y29">
-        <v>1</v>
-      </c>
-      <c r="Z29">
-        <v>1</v>
-      </c>
-      <c r="AA29">
-        <v>1</v>
-      </c>
-      <c r="AB29">
-        <v>0</v>
-      </c>
-      <c r="AC29">
-        <v>0</v>
-      </c>
-      <c r="AD29">
-        <v>1</v>
-      </c>
-      <c r="AE29">
-        <v>1</v>
-      </c>
-      <c r="AF29">
-        <v>1</v>
-      </c>
-      <c r="AG29" t="s">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>0</v>
+      </c>
+      <c r="B29" s="2">
+        <v>0</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0</v>
+      </c>
+      <c r="G29" s="2">
+        <v>1</v>
+      </c>
+      <c r="H29" s="2">
+        <v>0</v>
+      </c>
+      <c r="I29" s="2">
+        <v>1</v>
+      </c>
+      <c r="J29" s="2">
+        <v>0</v>
+      </c>
+      <c r="K29" s="2">
+        <v>1</v>
+      </c>
+      <c r="L29" s="2">
+        <v>0</v>
+      </c>
+      <c r="M29" s="2">
+        <v>0</v>
+      </c>
+      <c r="N29" s="2">
+        <v>0</v>
+      </c>
+      <c r="O29" s="2">
+        <v>1</v>
+      </c>
+      <c r="P29" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="2">
+        <v>0</v>
+      </c>
+      <c r="R29" s="2">
+        <v>0</v>
+      </c>
+      <c r="S29" s="2">
+        <v>0</v>
+      </c>
+      <c r="T29" s="2">
+        <v>0</v>
+      </c>
+      <c r="U29" s="2">
+        <v>0</v>
+      </c>
+      <c r="V29" s="2">
+        <v>0</v>
+      </c>
+      <c r="W29" s="2">
+        <v>0</v>
+      </c>
+      <c r="X29" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y29" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z29" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA29" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB29" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC29" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD29" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE29" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF29" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG29" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>1</v>
-      </c>
-      <c r="B31">
-        <v>0</v>
-      </c>
-      <c r="C31">
-        <v>0</v>
-      </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <v>0</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
-      <c r="G31">
-        <v>1</v>
-      </c>
-      <c r="H31">
-        <v>0</v>
-      </c>
-      <c r="I31">
-        <v>0</v>
-      </c>
-      <c r="J31">
-        <v>1</v>
-      </c>
-      <c r="K31">
-        <v>1</v>
-      </c>
-      <c r="L31">
-        <v>1</v>
-      </c>
-      <c r="M31">
-        <v>0</v>
-      </c>
-      <c r="N31">
-        <v>0</v>
-      </c>
-      <c r="O31">
-        <v>1</v>
-      </c>
-      <c r="P31">
-        <v>0</v>
-      </c>
-      <c r="Q31">
-        <v>0</v>
-      </c>
-      <c r="R31">
-        <v>0</v>
-      </c>
-      <c r="S31">
-        <v>0</v>
-      </c>
-      <c r="T31">
-        <v>0</v>
-      </c>
-      <c r="U31">
-        <v>1</v>
-      </c>
-      <c r="V31">
-        <v>0</v>
-      </c>
-      <c r="W31">
-        <v>0</v>
-      </c>
-      <c r="X31">
-        <v>0</v>
-      </c>
-      <c r="Y31">
-        <v>1</v>
-      </c>
-      <c r="Z31">
-        <v>1</v>
-      </c>
-      <c r="AA31">
-        <v>1</v>
-      </c>
-      <c r="AB31">
-        <v>0</v>
-      </c>
-      <c r="AC31">
-        <v>0</v>
-      </c>
-      <c r="AD31">
-        <v>0</v>
-      </c>
-      <c r="AE31">
-        <v>1</v>
-      </c>
-      <c r="AF31">
-        <v>1</v>
-      </c>
-      <c r="AG31" t="s">
+    <row r="30" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AG30" s="6"/>
+    </row>
+    <row r="31" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
+        <v>1</v>
+      </c>
+      <c r="B31" s="2">
+        <v>0</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0</v>
+      </c>
+      <c r="E31" s="2">
+        <v>0</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0</v>
+      </c>
+      <c r="G31" s="2">
+        <v>1</v>
+      </c>
+      <c r="H31" s="2">
+        <v>0</v>
+      </c>
+      <c r="I31" s="2">
+        <v>0</v>
+      </c>
+      <c r="J31" s="2">
+        <v>1</v>
+      </c>
+      <c r="K31" s="2">
+        <v>1</v>
+      </c>
+      <c r="L31" s="2">
+        <v>1</v>
+      </c>
+      <c r="M31" s="2">
+        <v>0</v>
+      </c>
+      <c r="N31" s="2">
+        <v>0</v>
+      </c>
+      <c r="O31" s="2">
+        <v>1</v>
+      </c>
+      <c r="P31" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="2">
+        <v>0</v>
+      </c>
+      <c r="R31" s="2">
+        <v>0</v>
+      </c>
+      <c r="S31" s="2">
+        <v>0</v>
+      </c>
+      <c r="T31" s="2">
+        <v>0</v>
+      </c>
+      <c r="U31" s="2">
+        <v>1</v>
+      </c>
+      <c r="V31" s="2">
+        <v>0</v>
+      </c>
+      <c r="W31" s="2">
+        <v>0</v>
+      </c>
+      <c r="X31" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y31" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z31" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA31" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB31" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC31" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD31" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE31" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF31" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG31" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="AI31" t="s">
-        <v>36</v>
-      </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>1</v>
-      </c>
-      <c r="B32">
-        <v>0</v>
-      </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-      <c r="E32">
-        <v>0</v>
-      </c>
-      <c r="F32">
-        <v>1</v>
-      </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
-      <c r="H32">
-        <v>0</v>
-      </c>
-      <c r="I32">
-        <v>0</v>
-      </c>
-      <c r="J32">
-        <v>1</v>
-      </c>
-      <c r="K32">
-        <v>1</v>
-      </c>
-      <c r="L32">
-        <v>1</v>
-      </c>
-      <c r="M32">
-        <v>0</v>
-      </c>
-      <c r="N32">
-        <v>0</v>
-      </c>
-      <c r="O32">
-        <v>1</v>
-      </c>
-      <c r="P32">
-        <v>0</v>
-      </c>
-      <c r="Q32">
-        <v>0</v>
-      </c>
-      <c r="R32">
-        <v>1</v>
-      </c>
-      <c r="S32">
-        <v>1</v>
-      </c>
-      <c r="T32">
-        <v>0</v>
-      </c>
-      <c r="U32">
-        <v>1</v>
-      </c>
-      <c r="V32">
-        <v>0</v>
-      </c>
-      <c r="W32">
-        <v>0</v>
-      </c>
-      <c r="X32">
-        <v>1</v>
-      </c>
-      <c r="Y32">
-        <v>0</v>
-      </c>
-      <c r="Z32">
-        <v>1</v>
-      </c>
-      <c r="AA32">
-        <v>1</v>
-      </c>
-      <c r="AB32">
-        <v>0</v>
-      </c>
-      <c r="AC32">
-        <v>0</v>
-      </c>
-      <c r="AD32">
-        <v>0</v>
-      </c>
-      <c r="AE32">
-        <v>1</v>
-      </c>
-      <c r="AF32">
-        <v>1</v>
-      </c>
-      <c r="AG32" t="s">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>1</v>
+      </c>
+      <c r="B32" s="2">
+        <v>0</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0</v>
+      </c>
+      <c r="E32" s="2">
+        <v>0</v>
+      </c>
+      <c r="F32" s="2">
+        <v>1</v>
+      </c>
+      <c r="G32" s="2">
+        <v>0</v>
+      </c>
+      <c r="H32" s="2">
+        <v>0</v>
+      </c>
+      <c r="I32" s="2">
+        <v>0</v>
+      </c>
+      <c r="J32" s="2">
+        <v>1</v>
+      </c>
+      <c r="K32" s="2">
+        <v>1</v>
+      </c>
+      <c r="L32" s="2">
+        <v>1</v>
+      </c>
+      <c r="M32" s="2">
+        <v>0</v>
+      </c>
+      <c r="N32" s="2">
+        <v>0</v>
+      </c>
+      <c r="O32" s="2">
+        <v>1</v>
+      </c>
+      <c r="P32" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="2">
+        <v>0</v>
+      </c>
+      <c r="R32" s="2">
+        <v>1</v>
+      </c>
+      <c r="S32" s="2">
+        <v>1</v>
+      </c>
+      <c r="T32" s="2">
+        <v>0</v>
+      </c>
+      <c r="U32" s="2">
+        <v>1</v>
+      </c>
+      <c r="V32" s="2">
+        <v>0</v>
+      </c>
+      <c r="W32" s="2">
+        <v>0</v>
+      </c>
+      <c r="X32" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y32" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z32" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA32" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB32" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC32" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD32" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE32" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF32" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG32" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>0</v>
-      </c>
-      <c r="B34">
-        <v>0</v>
-      </c>
-      <c r="C34">
-        <v>0</v>
-      </c>
-      <c r="D34">
-        <v>0</v>
-      </c>
-      <c r="E34">
-        <v>0</v>
-      </c>
-      <c r="F34">
-        <v>0</v>
-      </c>
-      <c r="G34">
-        <v>0</v>
-      </c>
-      <c r="H34">
-        <v>0</v>
-      </c>
-      <c r="I34">
-        <v>0</v>
-      </c>
-      <c r="J34">
-        <v>0</v>
-      </c>
-      <c r="K34">
-        <v>0</v>
-      </c>
-      <c r="L34">
-        <v>0</v>
-      </c>
-      <c r="M34">
-        <v>0</v>
-      </c>
-      <c r="N34">
-        <v>0</v>
-      </c>
-      <c r="O34">
-        <v>0</v>
-      </c>
-      <c r="P34">
-        <v>0</v>
-      </c>
-      <c r="Q34">
-        <v>0</v>
-      </c>
-      <c r="R34">
-        <v>0</v>
-      </c>
-      <c r="S34">
-        <v>0</v>
-      </c>
-      <c r="T34">
-        <v>0</v>
-      </c>
-      <c r="U34">
-        <v>0</v>
-      </c>
-      <c r="V34">
-        <v>0</v>
-      </c>
-      <c r="W34">
-        <v>0</v>
-      </c>
-      <c r="X34">
-        <v>0</v>
-      </c>
-      <c r="Y34">
-        <v>0</v>
-      </c>
-      <c r="Z34">
-        <v>1</v>
-      </c>
-      <c r="AA34">
-        <v>1</v>
-      </c>
-      <c r="AB34">
-        <v>1</v>
-      </c>
-      <c r="AC34">
-        <v>0</v>
-      </c>
-      <c r="AD34">
-        <v>0</v>
-      </c>
-      <c r="AE34">
-        <v>1</v>
-      </c>
-      <c r="AF34">
-        <v>1</v>
-      </c>
-      <c r="AG34" t="s">
+    <row r="33" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AG33" s="6"/>
+    </row>
+    <row r="34" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
+        <v>0</v>
+      </c>
+      <c r="B34" s="2">
+        <v>0</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0</v>
+      </c>
+      <c r="E34" s="2">
+        <v>0</v>
+      </c>
+      <c r="F34" s="2">
+        <v>0</v>
+      </c>
+      <c r="G34" s="2">
+        <v>0</v>
+      </c>
+      <c r="H34" s="2">
+        <v>0</v>
+      </c>
+      <c r="I34" s="2">
+        <v>0</v>
+      </c>
+      <c r="J34" s="2">
+        <v>0</v>
+      </c>
+      <c r="K34" s="2">
+        <v>0</v>
+      </c>
+      <c r="L34" s="2">
+        <v>0</v>
+      </c>
+      <c r="M34" s="2">
+        <v>0</v>
+      </c>
+      <c r="N34" s="2">
+        <v>0</v>
+      </c>
+      <c r="O34" s="2">
+        <v>0</v>
+      </c>
+      <c r="P34" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="2">
+        <v>0</v>
+      </c>
+      <c r="R34" s="2">
+        <v>0</v>
+      </c>
+      <c r="S34" s="2">
+        <v>0</v>
+      </c>
+      <c r="T34" s="2">
+        <v>0</v>
+      </c>
+      <c r="U34" s="2">
+        <v>0</v>
+      </c>
+      <c r="V34" s="2">
+        <v>0</v>
+      </c>
+      <c r="W34" s="2">
+        <v>0</v>
+      </c>
+      <c r="X34" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y34" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z34" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA34" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB34" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC34" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD34" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE34" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF34" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG34" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>0</v>
-      </c>
-      <c r="B35">
-        <v>0</v>
-      </c>
-      <c r="C35">
-        <v>0</v>
-      </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
-      <c r="E35">
-        <v>0</v>
-      </c>
-      <c r="F35">
-        <v>0</v>
-      </c>
-      <c r="G35">
-        <v>0</v>
-      </c>
-      <c r="H35">
-        <v>0</v>
-      </c>
-      <c r="I35">
-        <v>0</v>
-      </c>
-      <c r="J35">
-        <v>0</v>
-      </c>
-      <c r="K35">
-        <v>0</v>
-      </c>
-      <c r="L35">
-        <v>1</v>
-      </c>
-      <c r="M35">
-        <v>0</v>
-      </c>
-      <c r="N35">
-        <v>0</v>
-      </c>
-      <c r="O35">
-        <v>0</v>
-      </c>
-      <c r="P35">
-        <v>0</v>
-      </c>
-      <c r="Q35">
-        <v>0</v>
-      </c>
-      <c r="R35">
-        <v>0</v>
-      </c>
-      <c r="S35">
-        <v>0</v>
-      </c>
-      <c r="T35">
-        <v>0</v>
-      </c>
-      <c r="U35">
-        <v>0</v>
-      </c>
-      <c r="V35">
-        <v>0</v>
-      </c>
-      <c r="W35">
-        <v>0</v>
-      </c>
-      <c r="X35">
-        <v>0</v>
-      </c>
-      <c r="Y35">
-        <v>0</v>
-      </c>
-      <c r="Z35">
-        <v>1</v>
-      </c>
-      <c r="AA35">
-        <v>1</v>
-      </c>
-      <c r="AB35">
-        <v>1</v>
-      </c>
-      <c r="AC35">
-        <v>0</v>
-      </c>
-      <c r="AD35">
-        <v>0</v>
-      </c>
-      <c r="AE35">
-        <v>1</v>
-      </c>
-      <c r="AF35">
-        <v>1</v>
-      </c>
-      <c r="AG35" t="s">
+      <c r="A35" s="2">
+        <v>0</v>
+      </c>
+      <c r="B35" s="2">
+        <v>0</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0</v>
+      </c>
+      <c r="E35" s="2">
+        <v>0</v>
+      </c>
+      <c r="F35" s="2">
+        <v>0</v>
+      </c>
+      <c r="G35" s="2">
+        <v>0</v>
+      </c>
+      <c r="H35" s="2">
+        <v>0</v>
+      </c>
+      <c r="I35" s="2">
+        <v>0</v>
+      </c>
+      <c r="J35" s="2">
+        <v>0</v>
+      </c>
+      <c r="K35" s="2">
+        <v>0</v>
+      </c>
+      <c r="L35" s="2">
+        <v>1</v>
+      </c>
+      <c r="M35" s="2">
+        <v>0</v>
+      </c>
+      <c r="N35" s="2">
+        <v>0</v>
+      </c>
+      <c r="O35" s="2">
+        <v>0</v>
+      </c>
+      <c r="P35" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="2">
+        <v>0</v>
+      </c>
+      <c r="R35" s="2">
+        <v>0</v>
+      </c>
+      <c r="S35" s="2">
+        <v>0</v>
+      </c>
+      <c r="T35" s="2">
+        <v>0</v>
+      </c>
+      <c r="U35" s="2">
+        <v>0</v>
+      </c>
+      <c r="V35" s="2">
+        <v>0</v>
+      </c>
+      <c r="W35" s="2">
+        <v>0</v>
+      </c>
+      <c r="X35" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y35" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z35" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA35" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB35" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC35" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD35" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE35" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF35" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG35" s="6" t="s">
         <v>28</v>
       </c>
+    </row>
+    <row r="36" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AG36" s="6"/>
     </row>
     <row r="37" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>0</v>
-      </c>
-      <c r="B37">
-        <v>0</v>
-      </c>
-      <c r="C37">
-        <v>0</v>
-      </c>
-      <c r="D37">
-        <v>0</v>
-      </c>
-      <c r="E37">
-        <v>0</v>
-      </c>
-      <c r="F37">
-        <v>0</v>
-      </c>
-      <c r="G37">
-        <v>0</v>
-      </c>
-      <c r="H37">
-        <v>0</v>
-      </c>
-      <c r="I37">
-        <v>0</v>
-      </c>
-      <c r="J37">
-        <v>0</v>
-      </c>
-      <c r="K37">
-        <v>0</v>
-      </c>
-      <c r="L37">
-        <v>0</v>
-      </c>
-      <c r="M37">
-        <v>0</v>
-      </c>
-      <c r="N37">
-        <v>0</v>
-      </c>
-      <c r="O37">
-        <v>0</v>
-      </c>
-      <c r="P37">
-        <v>0</v>
-      </c>
-      <c r="Q37">
-        <v>0</v>
-      </c>
-      <c r="R37">
-        <v>0</v>
-      </c>
-      <c r="S37">
-        <v>0</v>
-      </c>
-      <c r="T37">
-        <v>0</v>
-      </c>
-      <c r="U37">
-        <v>0</v>
-      </c>
-      <c r="V37">
-        <v>0</v>
-      </c>
-      <c r="W37">
-        <v>0</v>
-      </c>
-      <c r="X37">
-        <v>0</v>
-      </c>
-      <c r="Y37">
-        <v>0</v>
-      </c>
-      <c r="Z37">
-        <v>0</v>
-      </c>
-      <c r="AA37">
-        <v>0</v>
-      </c>
-      <c r="AB37">
-        <v>0</v>
-      </c>
-      <c r="AC37">
-        <v>0</v>
-      </c>
-      <c r="AD37">
-        <v>0</v>
-      </c>
-      <c r="AE37">
-        <v>0</v>
-      </c>
-      <c r="AF37">
-        <v>0</v>
-      </c>
-      <c r="AG37" t="s">
+      <c r="A37" s="2">
+        <v>0</v>
+      </c>
+      <c r="B37" s="2">
+        <v>0</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0</v>
+      </c>
+      <c r="E37" s="2">
+        <v>0</v>
+      </c>
+      <c r="F37" s="2">
+        <v>0</v>
+      </c>
+      <c r="G37" s="2">
+        <v>0</v>
+      </c>
+      <c r="H37" s="2">
+        <v>0</v>
+      </c>
+      <c r="I37" s="2">
+        <v>0</v>
+      </c>
+      <c r="J37" s="2">
+        <v>0</v>
+      </c>
+      <c r="K37" s="2">
+        <v>0</v>
+      </c>
+      <c r="L37" s="2">
+        <v>0</v>
+      </c>
+      <c r="M37" s="2">
+        <v>0</v>
+      </c>
+      <c r="N37" s="2">
+        <v>0</v>
+      </c>
+      <c r="O37" s="2">
+        <v>0</v>
+      </c>
+      <c r="P37" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="2">
+        <v>0</v>
+      </c>
+      <c r="R37" s="2">
+        <v>0</v>
+      </c>
+      <c r="S37" s="2">
+        <v>0</v>
+      </c>
+      <c r="T37" s="2">
+        <v>0</v>
+      </c>
+      <c r="U37" s="2">
+        <v>0</v>
+      </c>
+      <c r="V37" s="2">
+        <v>0</v>
+      </c>
+      <c r="W37" s="2">
+        <v>0</v>
+      </c>
+      <c r="X37" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y37" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z37" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA37" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB37" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC37" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD37" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE37" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF37" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG37" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>0</v>
-      </c>
-      <c r="B39">
-        <v>0</v>
-      </c>
-      <c r="C39">
-        <v>1</v>
-      </c>
-      <c r="D39">
-        <v>1</v>
-      </c>
-      <c r="E39">
-        <v>0</v>
-      </c>
-      <c r="F39">
-        <v>0</v>
-      </c>
-      <c r="G39">
-        <v>0</v>
-      </c>
-      <c r="H39">
-        <v>0</v>
-      </c>
-      <c r="I39">
-        <v>0</v>
-      </c>
-      <c r="J39">
-        <v>0</v>
-      </c>
-      <c r="K39">
-        <v>1</v>
-      </c>
-      <c r="L39">
-        <v>0</v>
-      </c>
-      <c r="M39">
-        <v>0</v>
-      </c>
-      <c r="N39">
-        <v>0</v>
-      </c>
-      <c r="O39">
-        <v>0</v>
-      </c>
-      <c r="P39">
-        <v>0</v>
-      </c>
-      <c r="Q39">
-        <v>0</v>
-      </c>
-      <c r="R39">
-        <v>0</v>
-      </c>
-      <c r="S39">
-        <v>0</v>
-      </c>
-      <c r="T39">
-        <v>0</v>
-      </c>
-      <c r="U39">
-        <v>0</v>
-      </c>
-      <c r="V39">
-        <v>0</v>
-      </c>
-      <c r="W39">
-        <v>0</v>
-      </c>
-      <c r="X39">
-        <v>0</v>
-      </c>
-      <c r="Y39">
-        <v>0</v>
-      </c>
-      <c r="Z39">
-        <v>1</v>
-      </c>
-      <c r="AA39">
-        <v>1</v>
-      </c>
-      <c r="AB39">
-        <v>1</v>
-      </c>
-      <c r="AC39">
-        <v>0</v>
-      </c>
-      <c r="AD39">
-        <v>0</v>
-      </c>
-      <c r="AE39">
-        <v>1</v>
-      </c>
-      <c r="AF39">
-        <v>1</v>
-      </c>
-      <c r="AG39" t="s">
+    <row r="38" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AG38" s="6"/>
+    </row>
+    <row r="39" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="2">
+        <v>0</v>
+      </c>
+      <c r="B39" s="2">
+        <v>0</v>
+      </c>
+      <c r="C39" s="2">
+        <v>1</v>
+      </c>
+      <c r="D39" s="2">
+        <v>1</v>
+      </c>
+      <c r="E39" s="2">
+        <v>0</v>
+      </c>
+      <c r="F39" s="2">
+        <v>0</v>
+      </c>
+      <c r="G39" s="2">
+        <v>0</v>
+      </c>
+      <c r="H39" s="2">
+        <v>0</v>
+      </c>
+      <c r="I39" s="2">
+        <v>0</v>
+      </c>
+      <c r="J39" s="2">
+        <v>0</v>
+      </c>
+      <c r="K39" s="2">
+        <v>1</v>
+      </c>
+      <c r="L39" s="2">
+        <v>0</v>
+      </c>
+      <c r="M39" s="2">
+        <v>0</v>
+      </c>
+      <c r="N39" s="2">
+        <v>0</v>
+      </c>
+      <c r="O39" s="2">
+        <v>0</v>
+      </c>
+      <c r="P39" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q39" s="2">
+        <v>0</v>
+      </c>
+      <c r="R39" s="2">
+        <v>0</v>
+      </c>
+      <c r="S39" s="2">
+        <v>0</v>
+      </c>
+      <c r="T39" s="2">
+        <v>0</v>
+      </c>
+      <c r="U39" s="2">
+        <v>0</v>
+      </c>
+      <c r="V39" s="2">
+        <v>0</v>
+      </c>
+      <c r="W39" s="2">
+        <v>0</v>
+      </c>
+      <c r="X39" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y39" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z39" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA39" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB39" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC39" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD39" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE39" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF39" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG39" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="40" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>0</v>
-      </c>
-      <c r="B40">
-        <v>0</v>
-      </c>
-      <c r="C40">
-        <v>0</v>
-      </c>
-      <c r="D40">
-        <v>1</v>
-      </c>
-      <c r="E40">
-        <v>0</v>
-      </c>
-      <c r="F40">
-        <v>0</v>
-      </c>
-      <c r="G40">
-        <v>0</v>
-      </c>
-      <c r="H40">
-        <v>0</v>
-      </c>
-      <c r="I40">
-        <v>0</v>
-      </c>
-      <c r="J40">
-        <v>1</v>
-      </c>
-      <c r="K40">
-        <v>0</v>
-      </c>
-      <c r="L40">
-        <v>1</v>
-      </c>
-      <c r="M40">
-        <v>0</v>
-      </c>
-      <c r="N40">
-        <v>0</v>
-      </c>
-      <c r="O40">
-        <v>0</v>
-      </c>
-      <c r="P40">
-        <v>0</v>
-      </c>
-      <c r="Q40">
-        <v>0</v>
-      </c>
-      <c r="R40">
-        <v>0</v>
-      </c>
-      <c r="S40">
-        <v>0</v>
-      </c>
-      <c r="T40">
-        <v>0</v>
-      </c>
-      <c r="U40">
-        <v>0</v>
-      </c>
-      <c r="V40">
-        <v>0</v>
-      </c>
-      <c r="W40">
-        <v>0</v>
-      </c>
-      <c r="X40">
-        <v>0</v>
-      </c>
-      <c r="Y40">
-        <v>0</v>
-      </c>
-      <c r="Z40">
-        <v>1</v>
-      </c>
-      <c r="AA40">
-        <v>1</v>
-      </c>
-      <c r="AB40">
-        <v>1</v>
-      </c>
-      <c r="AC40">
-        <v>0</v>
-      </c>
-      <c r="AD40">
-        <v>0</v>
-      </c>
-      <c r="AE40">
-        <v>1</v>
-      </c>
-      <c r="AF40">
-        <v>1</v>
-      </c>
-      <c r="AG40" t="s">
+      <c r="A40" s="2">
+        <v>0</v>
+      </c>
+      <c r="B40" s="2">
+        <v>0</v>
+      </c>
+      <c r="C40" s="2">
+        <v>0</v>
+      </c>
+      <c r="D40" s="2">
+        <v>1</v>
+      </c>
+      <c r="E40" s="2">
+        <v>0</v>
+      </c>
+      <c r="F40" s="2">
+        <v>0</v>
+      </c>
+      <c r="G40" s="2">
+        <v>0</v>
+      </c>
+      <c r="H40" s="2">
+        <v>0</v>
+      </c>
+      <c r="I40" s="2">
+        <v>0</v>
+      </c>
+      <c r="J40" s="2">
+        <v>1</v>
+      </c>
+      <c r="K40" s="2">
+        <v>0</v>
+      </c>
+      <c r="L40" s="2">
+        <v>1</v>
+      </c>
+      <c r="M40" s="2">
+        <v>0</v>
+      </c>
+      <c r="N40" s="2">
+        <v>0</v>
+      </c>
+      <c r="O40" s="2">
+        <v>0</v>
+      </c>
+      <c r="P40" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="2">
+        <v>0</v>
+      </c>
+      <c r="R40" s="2">
+        <v>0</v>
+      </c>
+      <c r="S40" s="2">
+        <v>0</v>
+      </c>
+      <c r="T40" s="2">
+        <v>0</v>
+      </c>
+      <c r="U40" s="2">
+        <v>0</v>
+      </c>
+      <c r="V40" s="2">
+        <v>0</v>
+      </c>
+      <c r="W40" s="2">
+        <v>0</v>
+      </c>
+      <c r="X40" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y40" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z40" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA40" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB40" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC40" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD40" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE40" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF40" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG40" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>0</v>
-      </c>
-      <c r="B42">
-        <v>0</v>
-      </c>
-      <c r="C42">
-        <v>0</v>
-      </c>
-      <c r="D42">
-        <v>0</v>
-      </c>
-      <c r="E42">
-        <v>0</v>
-      </c>
-      <c r="F42">
-        <v>0</v>
-      </c>
-      <c r="G42">
-        <v>0</v>
-      </c>
-      <c r="H42">
-        <v>0</v>
-      </c>
-      <c r="I42">
-        <v>0</v>
-      </c>
-      <c r="J42">
-        <v>1</v>
-      </c>
-      <c r="K42">
-        <v>0</v>
-      </c>
-      <c r="L42">
-        <v>0</v>
-      </c>
-      <c r="M42">
-        <v>0</v>
-      </c>
-      <c r="N42">
-        <v>0</v>
-      </c>
-      <c r="O42">
-        <v>1</v>
-      </c>
-      <c r="P42">
-        <v>1</v>
-      </c>
-      <c r="Q42">
-        <v>0</v>
-      </c>
-      <c r="R42">
-        <v>0</v>
-      </c>
-      <c r="S42">
-        <v>0</v>
-      </c>
-      <c r="T42">
-        <v>1</v>
-      </c>
-      <c r="U42">
-        <v>0</v>
-      </c>
-      <c r="V42">
-        <v>0</v>
-      </c>
-      <c r="W42">
-        <v>1</v>
-      </c>
-      <c r="X42">
-        <v>0</v>
-      </c>
-      <c r="Y42">
-        <v>0</v>
-      </c>
-      <c r="Z42">
-        <v>1</v>
-      </c>
-      <c r="AA42">
-        <v>1</v>
-      </c>
-      <c r="AB42">
-        <v>1</v>
-      </c>
-      <c r="AC42">
-        <v>0</v>
-      </c>
-      <c r="AD42">
-        <v>0</v>
-      </c>
-      <c r="AE42">
-        <v>1</v>
-      </c>
-      <c r="AF42">
-        <v>1</v>
-      </c>
-      <c r="AG42" t="s">
+    <row r="41" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AG41" s="6"/>
+    </row>
+    <row r="42" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="2">
+        <v>0</v>
+      </c>
+      <c r="B42" s="2">
+        <v>0</v>
+      </c>
+      <c r="C42" s="2">
+        <v>0</v>
+      </c>
+      <c r="D42" s="2">
+        <v>0</v>
+      </c>
+      <c r="E42" s="2">
+        <v>0</v>
+      </c>
+      <c r="F42" s="2">
+        <v>0</v>
+      </c>
+      <c r="G42" s="2">
+        <v>0</v>
+      </c>
+      <c r="H42" s="2">
+        <v>0</v>
+      </c>
+      <c r="I42" s="2">
+        <v>0</v>
+      </c>
+      <c r="J42" s="2">
+        <v>1</v>
+      </c>
+      <c r="K42" s="2">
+        <v>0</v>
+      </c>
+      <c r="L42" s="2">
+        <v>0</v>
+      </c>
+      <c r="M42" s="2">
+        <v>0</v>
+      </c>
+      <c r="N42" s="2">
+        <v>0</v>
+      </c>
+      <c r="O42" s="2">
+        <v>1</v>
+      </c>
+      <c r="P42" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q42" s="2">
+        <v>0</v>
+      </c>
+      <c r="R42" s="2">
+        <v>0</v>
+      </c>
+      <c r="S42" s="2">
+        <v>0</v>
+      </c>
+      <c r="T42" s="2">
+        <v>1</v>
+      </c>
+      <c r="U42" s="2">
+        <v>0</v>
+      </c>
+      <c r="V42" s="2">
+        <v>0</v>
+      </c>
+      <c r="W42" s="2">
+        <v>1</v>
+      </c>
+      <c r="X42" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y42" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z42" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA42" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB42" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC42" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD42" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE42" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF42" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG42" s="6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="43" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>0</v>
-      </c>
-      <c r="B43">
-        <v>0</v>
-      </c>
-      <c r="C43">
-        <v>0</v>
-      </c>
-      <c r="D43">
-        <v>0</v>
-      </c>
-      <c r="E43">
-        <v>0</v>
-      </c>
-      <c r="F43">
-        <v>0</v>
-      </c>
-      <c r="G43">
-        <v>0</v>
-      </c>
-      <c r="H43">
-        <v>0</v>
-      </c>
-      <c r="I43">
-        <v>0</v>
-      </c>
-      <c r="J43">
-        <v>1</v>
-      </c>
-      <c r="K43">
-        <v>0</v>
-      </c>
-      <c r="L43">
-        <v>0</v>
-      </c>
-      <c r="M43">
-        <v>0</v>
-      </c>
-      <c r="N43">
-        <v>0</v>
-      </c>
-      <c r="O43">
-        <v>1</v>
-      </c>
-      <c r="P43">
-        <v>0</v>
-      </c>
-      <c r="Q43">
-        <v>0</v>
-      </c>
-      <c r="R43">
-        <v>1</v>
-      </c>
-      <c r="S43">
-        <v>0</v>
-      </c>
-      <c r="T43">
-        <v>1</v>
-      </c>
-      <c r="U43">
-        <v>0</v>
-      </c>
-      <c r="V43">
-        <v>0</v>
-      </c>
-      <c r="W43">
-        <v>1</v>
-      </c>
-      <c r="X43">
-        <v>0</v>
-      </c>
-      <c r="Y43">
-        <v>0</v>
-      </c>
-      <c r="Z43">
-        <v>1</v>
-      </c>
-      <c r="AA43">
-        <v>1</v>
-      </c>
-      <c r="AB43">
-        <v>1</v>
-      </c>
-      <c r="AC43">
-        <v>0</v>
-      </c>
-      <c r="AD43">
-        <v>0</v>
-      </c>
-      <c r="AE43">
-        <v>1</v>
-      </c>
-      <c r="AF43">
-        <v>1</v>
-      </c>
-      <c r="AG43" t="s">
+      <c r="A43" s="2">
+        <v>0</v>
+      </c>
+      <c r="B43" s="2">
+        <v>0</v>
+      </c>
+      <c r="C43" s="2">
+        <v>0</v>
+      </c>
+      <c r="D43" s="2">
+        <v>0</v>
+      </c>
+      <c r="E43" s="2">
+        <v>0</v>
+      </c>
+      <c r="F43" s="2">
+        <v>0</v>
+      </c>
+      <c r="G43" s="2">
+        <v>0</v>
+      </c>
+      <c r="H43" s="2">
+        <v>0</v>
+      </c>
+      <c r="I43" s="2">
+        <v>0</v>
+      </c>
+      <c r="J43" s="2">
+        <v>1</v>
+      </c>
+      <c r="K43" s="2">
+        <v>0</v>
+      </c>
+      <c r="L43" s="2">
+        <v>0</v>
+      </c>
+      <c r="M43" s="2">
+        <v>0</v>
+      </c>
+      <c r="N43" s="2">
+        <v>0</v>
+      </c>
+      <c r="O43" s="2">
+        <v>1</v>
+      </c>
+      <c r="P43" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q43" s="2">
+        <v>0</v>
+      </c>
+      <c r="R43" s="2">
+        <v>1</v>
+      </c>
+      <c r="S43" s="2">
+        <v>0</v>
+      </c>
+      <c r="T43" s="2">
+        <v>1</v>
+      </c>
+      <c r="U43" s="2">
+        <v>0</v>
+      </c>
+      <c r="V43" s="2">
+        <v>0</v>
+      </c>
+      <c r="W43" s="2">
+        <v>1</v>
+      </c>
+      <c r="X43" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y43" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z43" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA43" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB43" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC43" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD43" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE43" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF43" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG43" s="6" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AG44" s="6"/>
+    </row>
+    <row r="45" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="2">
+        <v>0</v>
+      </c>
+      <c r="B45" s="2">
+        <v>0</v>
+      </c>
+      <c r="C45" s="2">
+        <v>0</v>
+      </c>
+      <c r="D45" s="2">
+        <v>0</v>
+      </c>
+      <c r="E45" s="2">
+        <v>0</v>
+      </c>
+      <c r="F45" s="2">
+        <v>0</v>
+      </c>
+      <c r="G45" s="2">
+        <v>0</v>
+      </c>
+      <c r="H45" s="2">
+        <v>0</v>
+      </c>
+      <c r="I45" s="2">
+        <v>0</v>
+      </c>
+      <c r="J45" s="2">
+        <v>0</v>
+      </c>
+      <c r="K45" s="2">
+        <v>1</v>
+      </c>
+      <c r="L45" s="2">
+        <v>0</v>
+      </c>
+      <c r="M45" s="2">
+        <v>0</v>
+      </c>
+      <c r="N45" s="2">
+        <v>0</v>
+      </c>
+      <c r="O45" s="2">
+        <v>0</v>
+      </c>
+      <c r="P45" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q45" s="2">
+        <v>1</v>
+      </c>
+      <c r="R45" s="2">
+        <v>0</v>
+      </c>
+      <c r="S45" s="2">
+        <v>0</v>
+      </c>
+      <c r="T45" s="2">
+        <v>0</v>
+      </c>
+      <c r="U45" s="2">
+        <v>0</v>
+      </c>
+      <c r="V45" s="2">
+        <v>0</v>
+      </c>
+      <c r="W45" s="2">
+        <v>1</v>
+      </c>
+      <c r="X45" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y45" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z45" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA45" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB45" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC45" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD45" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE45" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF45" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG45" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="46" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="2">
+        <v>0</v>
+      </c>
+      <c r="B46" s="2">
+        <v>0</v>
+      </c>
+      <c r="C46" s="2">
+        <v>0</v>
+      </c>
+      <c r="D46" s="2">
+        <v>0</v>
+      </c>
+      <c r="E46" s="2">
+        <v>0</v>
+      </c>
+      <c r="F46" s="2">
+        <v>0</v>
+      </c>
+      <c r="G46" s="2">
+        <v>0</v>
+      </c>
+      <c r="H46" s="2">
+        <v>0</v>
+      </c>
+      <c r="I46" s="2">
+        <v>0</v>
+      </c>
+      <c r="J46" s="2">
+        <v>0</v>
+      </c>
+      <c r="K46" s="2">
+        <v>1</v>
+      </c>
+      <c r="L46" s="2">
+        <v>0</v>
+      </c>
+      <c r="M46" s="2">
+        <v>0</v>
+      </c>
+      <c r="N46" s="2">
+        <v>0</v>
+      </c>
+      <c r="O46" s="2">
+        <v>0</v>
+      </c>
+      <c r="P46" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q46" s="2">
+        <v>1</v>
+      </c>
+      <c r="R46" s="2">
+        <v>0</v>
+      </c>
+      <c r="S46" s="2">
+        <v>0</v>
+      </c>
+      <c r="T46" s="2">
+        <v>1</v>
+      </c>
+      <c r="U46" s="2">
+        <v>0</v>
+      </c>
+      <c r="V46" s="2">
+        <v>0</v>
+      </c>
+      <c r="W46" s="2">
+        <v>1</v>
+      </c>
+      <c r="X46" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y46" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z46" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA46" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB46" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC46" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD46" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE46" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF46" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG46" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>0</v>
+      </c>
+      <c r="B47" s="2">
+        <v>0</v>
+      </c>
+      <c r="C47" s="2">
+        <v>0</v>
+      </c>
+      <c r="D47" s="2">
+        <v>0</v>
+      </c>
+      <c r="E47" s="2">
+        <v>0</v>
+      </c>
+      <c r="F47" s="2">
+        <v>0</v>
+      </c>
+      <c r="G47" s="2">
+        <v>0</v>
+      </c>
+      <c r="H47" s="2">
+        <v>0</v>
+      </c>
+      <c r="I47" s="2">
+        <v>0</v>
+      </c>
+      <c r="J47" s="2">
+        <v>0</v>
+      </c>
+      <c r="K47" s="2">
+        <v>1</v>
+      </c>
+      <c r="L47" s="2">
+        <v>0</v>
+      </c>
+      <c r="M47" s="2">
+        <v>0</v>
+      </c>
+      <c r="N47" s="2">
+        <v>0</v>
+      </c>
+      <c r="O47" s="2">
+        <v>0</v>
+      </c>
+      <c r="P47" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q47" s="2">
+        <v>1</v>
+      </c>
+      <c r="R47" s="2">
+        <v>0</v>
+      </c>
+      <c r="S47" s="2">
+        <v>1</v>
+      </c>
+      <c r="T47" s="2">
+        <v>0</v>
+      </c>
+      <c r="U47" s="2">
+        <v>0</v>
+      </c>
+      <c r="V47" s="2">
+        <v>0</v>
+      </c>
+      <c r="W47" s="2">
+        <v>1</v>
+      </c>
+      <c r="X47" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y47" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z47" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA47" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB47" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC47" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD47" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE47" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF47" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG47" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="48" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AG48" s="6"/>
+    </row>
+    <row r="49" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="2">
+        <v>0</v>
+      </c>
+      <c r="B49" s="2">
+        <v>0</v>
+      </c>
+      <c r="C49" s="2">
+        <v>0</v>
+      </c>
+      <c r="D49" s="2">
+        <v>0</v>
+      </c>
+      <c r="E49" s="2">
+        <v>0</v>
+      </c>
+      <c r="F49" s="2">
+        <v>0</v>
+      </c>
+      <c r="G49" s="2">
+        <v>0</v>
+      </c>
+      <c r="H49" s="2">
+        <v>0</v>
+      </c>
+      <c r="I49" s="2">
+        <v>0</v>
+      </c>
+      <c r="J49" s="2">
+        <v>0</v>
+      </c>
+      <c r="K49" s="2">
+        <v>0</v>
+      </c>
+      <c r="L49" s="2">
+        <v>1</v>
+      </c>
+      <c r="M49" s="2">
+        <v>0</v>
+      </c>
+      <c r="N49" s="2">
+        <v>0</v>
+      </c>
+      <c r="O49" s="2">
+        <v>1</v>
+      </c>
+      <c r="P49" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q49" s="2">
+        <v>0</v>
+      </c>
+      <c r="R49" s="2">
+        <v>0</v>
+      </c>
+      <c r="S49" s="2">
+        <v>0</v>
+      </c>
+      <c r="T49" s="2">
+        <v>0</v>
+      </c>
+      <c r="U49" s="2">
+        <v>0</v>
+      </c>
+      <c r="V49" s="2">
+        <v>1</v>
+      </c>
+      <c r="W49" s="2">
+        <v>0</v>
+      </c>
+      <c r="X49" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y49" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z49" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA49" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB49" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC49" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD49" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE49" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF49" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG49" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="50" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="2">
+        <v>0</v>
+      </c>
+      <c r="B50" s="2">
+        <v>0</v>
+      </c>
+      <c r="C50" s="2">
+        <v>0</v>
+      </c>
+      <c r="D50" s="2">
+        <v>0</v>
+      </c>
+      <c r="E50" s="2">
+        <v>0</v>
+      </c>
+      <c r="F50" s="2">
+        <v>0</v>
+      </c>
+      <c r="G50" s="2">
+        <v>0</v>
+      </c>
+      <c r="H50" s="2">
+        <v>0</v>
+      </c>
+      <c r="I50" s="2">
+        <v>0</v>
+      </c>
+      <c r="J50" s="2">
+        <v>0</v>
+      </c>
+      <c r="K50" s="2">
+        <v>0</v>
+      </c>
+      <c r="L50" s="2">
+        <v>1</v>
+      </c>
+      <c r="M50" s="2">
+        <v>0</v>
+      </c>
+      <c r="N50" s="2">
+        <v>0</v>
+      </c>
+      <c r="O50" s="2">
+        <v>1</v>
+      </c>
+      <c r="P50" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q50" s="2">
+        <v>0</v>
+      </c>
+      <c r="R50" s="2">
+        <v>0</v>
+      </c>
+      <c r="S50" s="2">
+        <v>0</v>
+      </c>
+      <c r="T50" s="2">
+        <v>1</v>
+      </c>
+      <c r="U50" s="2">
+        <v>0</v>
+      </c>
+      <c r="V50" s="2">
+        <v>1</v>
+      </c>
+      <c r="W50" s="2">
+        <v>0</v>
+      </c>
+      <c r="X50" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y50" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z50" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA50" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB50" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC50" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD50" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE50" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF50" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG50" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="51" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>0</v>
+      </c>
+      <c r="B51" s="2">
+        <v>0</v>
+      </c>
+      <c r="C51" s="2">
+        <v>0</v>
+      </c>
+      <c r="D51" s="2">
+        <v>0</v>
+      </c>
+      <c r="E51" s="2">
+        <v>0</v>
+      </c>
+      <c r="F51" s="2">
+        <v>0</v>
+      </c>
+      <c r="G51" s="2">
+        <v>0</v>
+      </c>
+      <c r="H51" s="2">
+        <v>0</v>
+      </c>
+      <c r="I51" s="2">
+        <v>0</v>
+      </c>
+      <c r="J51" s="2">
+        <v>0</v>
+      </c>
+      <c r="K51" s="2">
+        <v>0</v>
+      </c>
+      <c r="L51" s="2">
+        <v>1</v>
+      </c>
+      <c r="M51" s="2">
+        <v>0</v>
+      </c>
+      <c r="N51" s="2">
+        <v>0</v>
+      </c>
+      <c r="O51" s="2">
+        <v>1</v>
+      </c>
+      <c r="P51" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q51" s="2">
+        <v>0</v>
+      </c>
+      <c r="R51" s="2">
+        <v>0</v>
+      </c>
+      <c r="S51" s="2">
+        <v>1</v>
+      </c>
+      <c r="T51" s="2">
+        <v>0</v>
+      </c>
+      <c r="U51" s="2">
+        <v>0</v>
+      </c>
+      <c r="V51" s="2">
+        <v>1</v>
+      </c>
+      <c r="W51" s="2">
+        <v>0</v>
+      </c>
+      <c r="X51" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y51" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z51" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA51" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB51" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC51" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD51" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE51" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF51" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG51" s="6" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -7334,7 +7944,7 @@
                     <xdr:col>34</xdr:col>
                     <xdr:colOff>495300</xdr:colOff>
                     <xdr:row>26</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -7355,8 +7965,8 @@
                   <to>
                     <xdr:col>34</xdr:col>
                     <xdr:colOff>495300</xdr:colOff>
-                    <xdr:row>27</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:row>26</xdr:row>
+                    <xdr:rowOff>190500</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -7377,8 +7987,8 @@
                   <to>
                     <xdr:col>34</xdr:col>
                     <xdr:colOff>495300</xdr:colOff>
-                    <xdr:row>28</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:row>27</xdr:row>
+                    <xdr:rowOff>190500</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -7422,7 +8032,7 @@
                     <xdr:col>34</xdr:col>
                     <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>31</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -7465,8 +8075,8 @@
                   <to>
                     <xdr:col>34</xdr:col>
                     <xdr:colOff>485775</xdr:colOff>
-                    <xdr:row>34</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
+                    <xdr:row>33</xdr:row>
+                    <xdr:rowOff>180975</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -7510,7 +8120,7 @@
                     <xdr:col>34</xdr:col>
                     <xdr:colOff>523875</xdr:colOff>
                     <xdr:row>39</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -7554,7 +8164,7 @@
                     <xdr:col>34</xdr:col>
                     <xdr:colOff>523875</xdr:colOff>
                     <xdr:row>41</xdr:row>
-                    <xdr:rowOff>180975</xdr:rowOff>
+                    <xdr:rowOff>171450</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -7576,7 +8186,7 @@
                     <xdr:col>34</xdr:col>
                     <xdr:colOff>533400</xdr:colOff>
                     <xdr:row>43</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -7598,7 +8208,7 @@
                     <xdr:col>34</xdr:col>
                     <xdr:colOff>504825</xdr:colOff>
                     <xdr:row>37</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>

</xml_diff>